<commit_message>
modulo relatorio geral pronto
</commit_message>
<xml_diff>
--- a/excel files/grade-exportacao (1).xlsx
+++ b/excel files/grade-exportacao (1).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Concluida</t>
   </si>
@@ -49,25 +49,46 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>fechado</t>
-  </si>
-  <si>
-    <t>Suporte Funcional</t>
+    <t>emaberto</t>
+  </si>
+  <si>
+    <t>Suporte Técnico</t>
   </si>
   <si>
     <t>Vitor Pereira Diogo</t>
   </si>
   <si>
-    <t>Oliveira Cardoso, Carvalho de Brito, Libardi Comar...</t>
-  </si>
-  <si>
-    <t>Deborah</t>
-  </si>
-  <si>
-    <t>25/06/2021 | 14:00:00 a 14:07:00</t>
-  </si>
-  <si>
-    <t>Disse que os nomes de 'Objetos' não estavam aparecendo. Expliquei a ela que os t...</t>
+    <t>Fiorot Advogados Associados</t>
+  </si>
+  <si>
+    <t>Márcia</t>
+  </si>
+  <si>
+    <t>28/06/2021 | 14:35:00 a 14:40:00</t>
+  </si>
+  <si>
+    <t>Informou que não consegue anexar nenhum arquivo no GED. Passou por e-mail uma me...</t>
+  </si>
+  <si>
+    <t>Incospal Construções Pré-Fabricadas S/A</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>28/06/2021 | 12:55:00 a 12:57:00</t>
+  </si>
+  <si>
+    <t>O e-mail foi enviado pelo cliente, encaminhei para Yasmim seguir com o procedime...</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>28/06/2021 | 11:08:00 a 11:14:00</t>
+  </si>
+  <si>
+    <t>Disse que não consegue abrir o Informa Diários. Pedi a ele que fizesse o procedi...</t>
   </si>
 </sst>
 </file>
@@ -75,10 +96,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -111,50 +132,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,8 +175,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,15 +192,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,6 +215,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -208,41 +261,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -255,25 +276,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,157 +444,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,6 +475,30 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,6 +525,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,168 +567,135 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -683,10 +704,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1037,23 +1058,23 @@
     <outlinePr showOutlineSymbols="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="9.85714285714286"/>
     <col min="2" max="2" width="7.28571428571429"/>
-    <col min="3" max="3" width="16.4285714285714"/>
+    <col min="3" max="3" width="14.5714285714286"/>
     <col min="4" max="4" width="17.1428571428571"/>
-    <col min="5" max="5" width="41.1428571428571"/>
-    <col min="6" max="6" width="8.14285714285714"/>
+    <col min="5" max="5" width="39.4285714285714"/>
+    <col min="6" max="6" width="8"/>
     <col min="7" max="7" width="13.5714285714286"/>
     <col min="8" max="8" width="28.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="11.7142857142857" customWidth="1" outlineLevel="3" collapsed="1"/>
+    <col min="9" max="9" width="11.7142857142857"/>
     <col min="10" max="10" width="8.14285714285714"/>
     <col min="11" max="11" width="41.1428571428571"/>
   </cols>
@@ -1098,7 +1119,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3">
-        <v>22648</v>
+        <v>22658</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -1113,39 +1134,109 @@
         <v>15</v>
       </c>
       <c r="G2" s="4">
-        <v>44372</v>
+        <v>44375</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" ht="13.5" spans="1:11">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+    <row r="3" ht="27" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>22657</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4">
+        <v>44375</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="I3" s="2">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" ht="27" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>22657</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="4">
+        <v>44375</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" ht="13.5" spans="1:11">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
   </sheetData>
   <sheetProtection objects="1" scenarios="1"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="22648"/>
-    <hyperlink ref="E2" r:id="rId2" display="Oliveira Cardoso, Carvalho de Brito, Libardi Comar..."/>
+    <hyperlink ref="B2" r:id="rId1" display="22658"/>
+    <hyperlink ref="E2" r:id="rId2" display="Fiorot Advogados Associados"/>
+    <hyperlink ref="B3" r:id="rId3" display="22657"/>
+    <hyperlink ref="E3" r:id="rId4" display="Incospal Construções Pré-Fabricadas S/A"/>
+    <hyperlink ref="B4" r:id="rId3" display="22657"/>
+    <hyperlink ref="E4" r:id="rId4" display="Incospal Construções Pré-Fabricadas S/A"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>